<commit_message>
add grainsize to figures
</commit_message>
<xml_diff>
--- a/raw/dating/US-EPA-WHETS_Pb-Cs_Models_rplum_23.2.8.xlsx
+++ b/raw/dating/US-EPA-WHETS_Pb-Cs_Models_rplum_23.2.8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15033\Dropbox\Collaborations\Autumn_Oczkowski\2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/balint_sawyer_epa_gov/Documents/Profile/Documents/Sawyer Balint/RStudio/wickford_cores/raw/dating/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF9CD8E-ED37-459D-9739-091C3ADCF59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{EEF9CD8E-ED37-459D-9739-091C3ADCF59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE908882-BBAC-4933-9744-4855D0284E9F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{D4AB0736-7849-43AD-AFF9-6DCFB631629C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D4AB0736-7849-43AD-AFF9-6DCFB631629C}"/>
   </bookViews>
   <sheets>
     <sheet name="read.me" sheetId="5" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>depth</t>
   </si>
@@ -94,10 +94,13 @@
     <t>cm, bottom of sediment unit</t>
   </si>
   <si>
-    <t xml:space="preserve">note: I have incorporated the estimated 10 cm of erosion into this core by adding 10 cm to the top. So, the first actual unit of your core is depth 12 (the bottom of your 0-2 cm unit). </t>
+    <t>The following pages report the chronological models developed using rplum (https://cran.r-project.org/web/packages/rplum/index.html; for further details on plum see Aquino-Lopez et al., 2018, https://doi.org/10.1007/s13253-018-0328-7; ) applied to Pb-210ex and Cs-137 gamma spectrometry results on your cores. See explanations for each field below.</t>
   </si>
   <si>
-    <t>The following pages report the chronological models developed using rplum (https://cran.r-project.org/web/packages/rplum/index.html; for further details on plum see Aquino-Lopez et al., 2018, https://doi.org/10.1007/s13253-018-0328-7; ) applied to Pb-210ex and Cs-137 gamma spectrometry results on your cores. See explanations for each field below.</t>
+    <t>end.pb</t>
+  </si>
+  <si>
+    <t>cs.peak</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -220,9 +223,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -243,13 +243,15 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="1" xr16:uid="{458F23C0-68B5-4BEE-9A65-86783C6367C3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="8" unboundColumnsRight="2">
+    <queryTableFields count="7">
       <queryTableField id="1" name="depth" tableColumnId="1"/>
       <queryTableField id="2" name="min" tableColumnId="2"/>
       <queryTableField id="3" name="max" tableColumnId="3"/>
       <queryTableField id="4" name="median" tableColumnId="4"/>
       <queryTableField id="5" name="mean" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -257,13 +259,15 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="3" xr16:uid="{9217E630-6646-4852-8659-56C176BB9B90}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="8" unboundColumnsRight="2">
+    <queryTableFields count="7">
       <queryTableField id="1" name="depth" tableColumnId="1"/>
       <queryTableField id="2" name="min" tableColumnId="2"/>
       <queryTableField id="3" name="max" tableColumnId="3"/>
       <queryTableField id="4" name="median" tableColumnId="4"/>
       <queryTableField id="5" name="mean" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -271,55 +275,63 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="6" xr16:uid="{E1880936-9251-4FA0-9B41-DD346C76B836}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="8" unboundColumnsRight="2">
+    <queryTableFields count="7">
       <queryTableField id="1" name="depth" tableColumnId="1"/>
       <queryTableField id="2" name="min" tableColumnId="2"/>
       <queryTableField id="3" name="max" tableColumnId="3"/>
       <queryTableField id="4" name="median" tableColumnId="4"/>
       <queryTableField id="5" name="mean" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
+      <queryTableField id="7" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{48FB7691-270C-421C-AD5E-EA9C07F4BA26}" name="AC2_2_23_51_ages" displayName="AC2_2_23_51_ages" ref="A1:E52" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E52" xr:uid="{48FB7691-270C-421C-AD5E-EA9C07F4BA26}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{48FB7691-270C-421C-AD5E-EA9C07F4BA26}" name="AC2_2_23_51_ages" displayName="AC2_2_23_51_ages" ref="A1:G52" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G52" xr:uid="{48FB7691-270C-421C-AD5E-EA9C07F4BA26}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C828BFDE-1982-4E13-BA73-F67FA171E821}" uniqueName="1" name="depth" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{2C37D99F-B691-4505-83D7-81AE4C81406C}" uniqueName="2" name="min" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{1AA30063-A5A0-43A2-B96D-8EEEA00D9909}" uniqueName="3" name="max" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{1DF1A727-1C02-4271-B75E-D5E65F9B4C87}" uniqueName="4" name="median" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{F7A5B097-6CCA-4A9F-98D6-02B37AE1754F}" uniqueName="5" name="mean" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{758857CA-E368-4DC4-AB0C-8A7ADFAD4545}" uniqueName="6" name="end.pb" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{8E3B3BA4-87DD-452F-8BFC-2707ABF28A12}" uniqueName="7" name="cs.peak" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{377B7714-788B-4998-A03E-AD7FC61D35F6}" name="M6_2_23_51_ages" displayName="M6_2_23_51_ages" ref="A1:E52" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E52" xr:uid="{377B7714-788B-4998-A03E-AD7FC61D35F6}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{377B7714-788B-4998-A03E-AD7FC61D35F6}" name="M6_2_23_51_ages" displayName="M6_2_23_51_ages" ref="A1:G52" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G52" xr:uid="{377B7714-788B-4998-A03E-AD7FC61D35F6}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D3027317-1C76-475E-AC1E-2140016F15AD}" uniqueName="1" name="depth" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{7CF8D3DB-815E-460F-A6F3-42C826B6AFBC}" uniqueName="2" name="min" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{3C15FD32-E296-4381-ADB7-AC96FC2F2BA3}" uniqueName="3" name="max" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{FBD77300-CEFE-4013-AAF1-A426266286AB}" uniqueName="4" name="median" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{D7B04F90-EA55-40B9-BFA2-74478D84E1DD}" uniqueName="5" name="mean" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{A90867BA-FE89-40C1-9B6A-A8FCD266E091}" uniqueName="6" name="end.pb" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{70630E86-CCD8-4748-9DC6-CC9B83B6BE79}" uniqueName="7" name="cs.peak" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7E0EF347-AFD9-4D69-81F9-656C7ED240EB}" name="S3_2_23_10cm_erosion_55_ages" displayName="S3_2_23_10cm_erosion_55_ages" ref="A1:E56" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E56" xr:uid="{7E0EF347-AFD9-4D69-81F9-656C7ED240EB}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7E0EF347-AFD9-4D69-81F9-656C7ED240EB}" name="S3_2_23_10cm_erosion_55_ages" displayName="S3_2_23_10cm_erosion_55_ages" ref="A1:G56" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G56" xr:uid="{7E0EF347-AFD9-4D69-81F9-656C7ED240EB}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FD0A2ABF-4E4B-484A-BD1C-B52C100DC5B6}" uniqueName="1" name="depth" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{CFB9A7F7-4DC2-4745-B63D-7ECFE4BB5B30}" uniqueName="2" name="min" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{12E7A32A-4056-4AF4-9DB5-ACAA38C3E73D}" uniqueName="3" name="max" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{8239BF33-09F7-4818-85B4-1B5B9C8A23FB}" uniqueName="4" name="median" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{B0391513-5980-4DE2-82B2-B069A3B05B1A}" uniqueName="5" name="mean" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{739EB5C9-ACBD-49B9-AC1D-95F9089ABBC8}" uniqueName="6" name="end.pb" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{53D7D2B4-FF70-4869-B050-E1713AAD20C3}" uniqueName="7" name="cs.peak" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,33 +640,33 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="1" customWidth="1"/>
-    <col min="6" max="10" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="23.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.54296875" style="1" customWidth="1"/>
+    <col min="6" max="10" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -671,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -704,19 +716,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21317EB1-1EBE-48E4-9560-774B4AEC4EDB}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -732,8 +746,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -750,7 +770,7 @@
         <v>2019.9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -767,7 +787,7 @@
         <v>2016.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -784,7 +804,7 @@
         <v>2012.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -801,7 +821,7 @@
         <v>2005.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -818,7 +838,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -835,7 +855,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -852,7 +872,7 @@
         <v>1988.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -869,7 +889,7 @@
         <v>1983.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -886,7 +906,7 @@
         <v>1978.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -903,7 +923,7 @@
         <v>1973.7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -919,8 +939,11 @@
       <c r="E12">
         <v>1968.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -937,7 +960,7 @@
         <v>1962.9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -954,7 +977,7 @@
         <v>1956.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -971,7 +994,7 @@
         <v>1950.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -988,7 +1011,7 @@
         <v>1943.6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1005,7 +1028,7 @@
         <v>1937.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1022,7 +1045,7 @@
         <v>1931.2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1039,7 +1062,7 @@
         <v>1925.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1056,7 +1079,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1073,7 +1096,7 @@
         <v>1912.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>1906.1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1107,7 +1130,7 @@
         <v>1899.7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1124,7 +1147,7 @@
         <v>1893.4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1141,7 +1164,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1158,7 +1181,7 @@
         <v>1880.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1175,7 +1198,7 @@
         <v>1874.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1192,7 +1215,7 @@
         <v>1868.3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1209,7 +1232,7 @@
         <v>1862.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1226,7 +1249,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1243,7 +1266,7 @@
         <v>1849.9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1260,7 +1283,7 @@
         <v>1843.8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1277,7 +1300,7 @@
         <v>1837.6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1294,7 +1317,7 @@
         <v>1831.4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1311,7 +1334,7 @@
         <v>1825.3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1328,7 +1351,7 @@
         <v>1819.2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1345,7 +1368,7 @@
         <v>1812.9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1362,7 +1385,7 @@
         <v>1806.7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1379,7 +1402,7 @@
         <v>1800.5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1395,8 +1418,11 @@
       <c r="E40">
         <v>1794.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1413,7 +1439,7 @@
         <v>1788.3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1430,7 +1456,7 @@
         <v>1782.3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1447,7 +1473,7 @@
         <v>1776.1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1464,7 +1490,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1481,7 +1507,7 @@
         <v>1763.9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1498,7 +1524,7 @@
         <v>1757.6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1515,7 +1541,7 @@
         <v>1751.3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1532,7 +1558,7 @@
         <v>1745.1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1549,7 +1575,7 @@
         <v>1738.9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1566,7 +1592,7 @@
         <v>1732.6</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1583,7 +1609,7 @@
         <v>1726.3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1610,21 +1636,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D47269D-B431-4CFC-8E7C-EA9C54D9147C}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1640,8 +1666,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1658,7 +1690,7 @@
         <v>2021.2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1675,7 +1707,7 @@
         <v>2017.7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1692,7 +1724,7 @@
         <v>2013.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1709,7 +1741,7 @@
         <v>2007.7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1726,7 +1758,7 @@
         <v>2001.7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1743,7 +1775,7 @@
         <v>1998.7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1760,7 +1792,7 @@
         <v>1995.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1777,7 +1809,7 @@
         <v>1992.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1794,7 +1826,7 @@
         <v>1988.1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1811,7 +1843,7 @@
         <v>1983.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1828,7 +1860,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1845,7 +1877,7 @@
         <v>1971.8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1862,7 +1894,7 @@
         <v>1965.3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1879,7 +1911,7 @@
         <v>1958.4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1895,8 +1927,11 @@
       <c r="E16">
         <v>1951.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1913,7 +1948,7 @@
         <v>1945.6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1930,7 +1965,7 @@
         <v>1939.2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1947,7 +1982,7 @@
         <v>1933.4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1964,7 +1999,7 @@
         <v>1927.6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1981,7 +2016,7 @@
         <v>1920.6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1998,7 +2033,7 @@
         <v>1913.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2015,7 +2050,7 @@
         <v>1906.9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2032,7 +2067,7 @@
         <v>1900.3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2049,7 +2084,7 @@
         <v>1893.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2066,7 +2101,7 @@
         <v>1886.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2083,7 +2118,7 @@
         <v>1880.2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2100,7 +2135,7 @@
         <v>1873.9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2117,7 +2152,7 @@
         <v>1867.4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2134,7 +2169,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2151,7 +2186,7 @@
         <v>1854.3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2168,7 +2203,7 @@
         <v>1847.7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2185,7 +2220,7 @@
         <v>1841.1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2202,7 +2237,7 @@
         <v>1834.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2219,7 +2254,7 @@
         <v>1827.8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2236,7 +2271,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2253,7 +2288,7 @@
         <v>1814.3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2270,7 +2305,7 @@
         <v>1807.6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2287,7 +2322,7 @@
         <v>1800.9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2303,8 +2338,11 @@
       <c r="E40">
         <v>1794.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2321,7 +2359,7 @@
         <v>1787.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2338,7 +2376,7 @@
         <v>1780.9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2355,7 +2393,7 @@
         <v>1774.4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2372,7 +2410,7 @@
         <v>1767.6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2389,7 +2427,7 @@
         <v>1760.9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2406,7 +2444,7 @@
         <v>1754.1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2423,7 +2461,7 @@
         <v>1747.4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2440,7 +2478,7 @@
         <v>1740.8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2457,7 +2495,7 @@
         <v>1734.4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2474,7 +2512,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2491,7 +2529,7 @@
         <v>1721.6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2518,21 +2556,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF19377-AB39-4C2E-9FEE-45E1788CAD04}">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2548,8 +2586,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2565,18 +2609,8 @@
       <c r="E2">
         <v>2021.2</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2592,16 +2626,8 @@
       <c r="E3">
         <v>2015.4</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2617,16 +2643,8 @@
       <c r="E4">
         <v>2010.2</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2643,7 +2661,7 @@
         <v>2005.4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2660,7 +2678,7 @@
         <v>2000.6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2677,7 +2695,7 @@
         <v>1995.8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2694,7 +2712,7 @@
         <v>1991.1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2711,7 +2729,7 @@
         <v>1986.5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2728,7 +2746,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2745,7 +2763,7 @@
         <v>1977.7</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2762,7 +2780,7 @@
         <v>1973.5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2779,7 +2797,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2795,8 +2813,11 @@
       <c r="E14">
         <v>1965.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2813,7 +2834,7 @@
         <v>1959.8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2830,7 +2851,7 @@
         <v>1952.3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2847,7 +2868,7 @@
         <v>1945.8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2864,7 +2885,7 @@
         <v>1939.4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2881,7 +2902,7 @@
         <v>1932.3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2898,7 +2919,7 @@
         <v>1925.1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2915,7 +2936,7 @@
         <v>1917.9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2932,7 +2953,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2949,7 +2970,7 @@
         <v>1904.7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2966,7 +2987,7 @@
         <v>1898.7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2983,7 +3004,7 @@
         <v>1892.8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3000,7 +3021,7 @@
         <v>1886.9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3017,7 +3038,7 @@
         <v>1880.7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3034,7 +3055,7 @@
         <v>1874.1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3051,7 +3072,7 @@
         <v>1867.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3068,7 +3089,7 @@
         <v>1860.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3085,7 +3106,7 @@
         <v>1853.3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3102,7 +3123,7 @@
         <v>1846.4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3119,7 +3140,7 @@
         <v>1839.8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3136,7 +3157,7 @@
         <v>1833.2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3153,7 +3174,7 @@
         <v>1826.6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3170,7 +3191,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3187,7 +3208,7 @@
         <v>1813.5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3204,7 +3225,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3221,7 +3242,7 @@
         <v>1800.5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3238,7 +3259,7 @@
         <v>1793.9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3255,7 +3276,7 @@
         <v>1787.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3272,7 +3293,7 @@
         <v>1781.1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3289,7 +3310,7 @@
         <v>1774.7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3305,8 +3326,11 @@
       <c r="E44">
         <v>1768.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3323,7 +3347,7 @@
         <v>1761.6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3340,7 +3364,7 @@
         <v>1755.1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3357,7 +3381,7 @@
         <v>1748.4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3374,7 +3398,7 @@
         <v>1741.7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3391,7 +3415,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3408,7 +3432,7 @@
         <v>1728.4</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3425,7 +3449,7 @@
         <v>1721.8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3442,7 +3466,7 @@
         <v>1715.3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3459,7 +3483,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3476,7 +3500,7 @@
         <v>1702.8</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3493,7 +3517,7 @@
         <v>1696.7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3511,9 +3535,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G2:N4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>